<commit_message>
Revert "noticeList db 수정"
This reverts commit 7c7c04c66328be6c13a3479e573913c8b1e59d02.
</commit_message>
<xml_diff>
--- a/어쩌다리그 화면설계.xlsx
+++ b/어쩌다리그 화면설계.xlsx
@@ -446,6 +446,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -459,22 +468,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -10249,112 +10249,112 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44224</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:9" ht="47.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:9" ht="38.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:9" ht="37" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="42.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:9" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="7:9" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="7:9" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="7:9" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="7:9" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="7:9" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="7:9" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="7:9" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="7:9" x14ac:dyDescent="0.45">
@@ -10419,13 +10419,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="G2:H2"/>
@@ -10440,6 +10433,13 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10491,49 +10491,49 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44224</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" ht="76" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G11" s="11"/>
@@ -10603,25 +10603,25 @@
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44224</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" s="14" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10678,21 +10678,21 @@
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44224</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10748,21 +10748,21 @@
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44224</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10819,21 +10819,21 @@
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44226</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10889,21 +10889,21 @@
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="16" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44226</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10958,21 +10958,21 @@
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44224</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="15" t="s">
@@ -11000,21 +11000,21 @@
       <c r="A33" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
       <c r="E33" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F33" s="13">
         <v>44224</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="19"/>
+      <c r="H33" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -11033,7 +11033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
@@ -11072,21 +11072,21 @@
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="16" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44226</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
@@ -11114,21 +11114,21 @@
       <c r="A21" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
       <c r="E21" s="16" t="s">
         <v>4</v>
       </c>
       <c r="F21" s="13">
         <v>44226</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="19"/>
+      <c r="H21" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -11186,33 +11186,33 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44224</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" ht="36.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G6" s="5"/>
@@ -11311,21 +11311,21 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44224</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G3" s="8"/>
@@ -11460,21 +11460,21 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44222</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G3" s="8"/>
@@ -11570,21 +11570,21 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44222</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G3" s="8"/>
@@ -11692,21 +11692,21 @@
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44224</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G3" s="8"/>
@@ -11838,21 +11838,21 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44224</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G3" s="8"/>
@@ -11984,25 +11984,25 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44222</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G4" s="9"/>
@@ -12074,145 +12074,145 @@
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="13">
         <v>44222</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="19"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
     </row>
     <row r="34" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
     </row>
     <row r="35" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
     </row>
     <row r="36" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
     </row>
     <row r="37" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
     </row>
     <row r="38" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
     </row>
     <row r="39" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
     </row>
     <row r="40" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
     </row>
     <row r="41" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
     </row>
     <row r="42" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
     </row>
     <row r="43" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
     </row>
     <row r="44" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
     </row>
     <row r="45" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
     </row>
     <row r="46" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
     </row>
     <row r="47" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
     </row>
     <row r="48" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -12273,21 +12273,21 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="13">
         <v>44222</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G3" s="8"/>

</xml_diff>